<commit_message>
Excel und Relaxivität neu -1
</commit_message>
<xml_diff>
--- a/Auswertung-MR/Excel/T1T2-Zeiten.xlsx
+++ b/Auswertung-MR/Excel/T1T2-Zeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Dokumente\Studium\Konstanz\7. Semester\FP\EFNMR-Remote\Auswertung-MR\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9316F701-C0A9-40D3-82FD-957E05B75D37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083A6A23-2F5B-4031-9EB0-C7F0D41701C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7164" yWindow="4248" windowWidth="12084" windowHeight="7920" xr2:uid="{A3CF1ACE-D739-42DC-9CD4-6918666B986E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Relaxationszeiten</t>
   </si>
@@ -114,6 +114,15 @@
   </si>
   <si>
     <t>Mn</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>u(1/t1)</t>
+  </si>
+  <si>
+    <t>u(1/t2)</t>
   </si>
 </sst>
 </file>
@@ -121,9 +130,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +142,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -158,11 +181,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -479,12 +504,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317E1452-D344-4788-8BB8-D10CA50AF815}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
@@ -776,12 +803,25 @@
         <v>5.4700000000000001E-5</v>
       </c>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="D18" t="s">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F18" t="s">
+      <c r="D18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="I18" t="s">
         <v>19</v>
@@ -802,40 +842,58 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D19">
+      <c r="C19" s="4">
         <f>1/D8</f>
         <v>4.5465705218553646E-4</v>
       </c>
-      <c r="F19">
+      <c r="D19" s="4">
+        <f>(1/D8^2)*E8</f>
+        <v>6.2572035725388004E-10</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5">
         <f>1/F8</f>
         <v>5.2602232438744704E-4</v>
       </c>
-    </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
+      <c r="G19" s="5">
+        <f>(1/F8^2)*G8</f>
+        <v>2.4855914805279351E-5</v>
+      </c>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D20">
+      <c r="C20" s="4">
         <f>1/D2</f>
         <v>7.1692810644948533E-4</v>
       </c>
-      <c r="E20">
+      <c r="D20" s="4">
+        <f>(1/D2^2)*E2</f>
+        <v>5.4225513485719294E-10</v>
+      </c>
+      <c r="E20" s="4">
         <f>K2</f>
         <v>0.5</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="5">
         <f>1/F2</f>
         <v>8.2269993665210492E-4</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="5">
+        <f>(1/F2^2)*G2</f>
+        <v>1.7117161848056976E-10</v>
+      </c>
+      <c r="H20" s="5">
         <v>0.5</v>
       </c>
       <c r="I20" s="2">
-        <f>(D20-$D$19)/E20</f>
+        <f>(C20-$C$19)/E20</f>
         <v>5.2454210852789774E-4</v>
       </c>
       <c r="J20" s="2">
@@ -846,80 +904,96 @@
         <v>0.5</v>
       </c>
       <c r="L20" s="3">
-        <f>(F20-$D$19)/G20</f>
+        <f>(F20-$C$19)/H20</f>
         <v>7.3608576893313693E-4</v>
       </c>
       <c r="M20" s="3">
-        <f>SQRT(((1/(F2^2*G20))*G2)^2+((1/($D$8^2*G20))*$E$8)^2)</f>
+        <f>SQRT(((1/(F2^2*H20))*G2)^2+((1/($D$8^2*H20))*$E$8)^2)</f>
         <v>1.2974215790639232E-9</v>
       </c>
       <c r="N20">
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D21">
+      <c r="C21" s="4">
         <f>1/D3</f>
         <v>9.9661152082918089E-4</v>
       </c>
-      <c r="E21">
+      <c r="D21" s="4">
+        <f t="shared" ref="D21:D23" si="2">(1/D3^2)*E3</f>
+        <v>4.8181806732532946E-10</v>
+      </c>
+      <c r="E21" s="4">
         <f>K3</f>
         <v>1</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="5">
         <f>1/F3</f>
         <v>9.3769926109298226E-4</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="5">
+        <f t="shared" ref="G21:G24" si="3">(1/F3^2)*G3</f>
+        <v>2.304592629050585E-10</v>
+      </c>
+      <c r="H21" s="5">
         <v>1</v>
       </c>
       <c r="I21" s="2">
-        <f>(D21-$D$19)/E21</f>
+        <f>(C21-$C$19)/E21</f>
         <v>5.4195446864364438E-4</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" ref="J21:J24" si="2">SQRT(((1/(D3^2*E21))*E3)^2+((1/($D$8^2*E21))*$E$8)^2)</f>
+        <f>SQRT(((1/(D3^2*E21))*E3)^2+((1/($D$8^2*E21))*$E$8)^2)</f>
         <v>7.8973072340072915E-10</v>
       </c>
       <c r="K21">
         <v>1</v>
       </c>
       <c r="L21" s="3">
-        <f>(F21-$D$19)/G21</f>
+        <f>(F21-$C$19)/H21</f>
         <v>4.830422089074458E-4</v>
       </c>
       <c r="M21" s="3">
-        <f>SQRT(((1/(F3^2*G21))*G3)^2+((1/($D$8^2*G21))*$E$8)^2)</f>
+        <f>SQRT(((1/(F3^2*H21))*G3)^2+((1/($D$8^2*H21))*$E$8)^2)</f>
         <v>6.6681139562897853E-10</v>
       </c>
       <c r="N21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D22">
+      <c r="C22" s="4">
         <f>1/D4</f>
         <v>1.5459558567764654E-3</v>
       </c>
-      <c r="E22">
+      <c r="D22" s="4">
+        <f t="shared" si="2"/>
+        <v>1.7097913422419814E-4</v>
+      </c>
+      <c r="E22" s="4">
         <f>K4</f>
         <v>2</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="5">
         <f>1/F4</f>
         <v>1.3361767173879348E-3</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="5">
+        <f t="shared" si="3"/>
+        <v>3.4582582423135492E-10</v>
+      </c>
+      <c r="H22" s="5">
         <v>2</v>
       </c>
       <c r="I22" s="2">
-        <f>(D22-$D$19)/E22</f>
+        <f>(C22-$C$19)/E22</f>
         <v>5.4564940229546446E-4</v>
       </c>
       <c r="J22" s="2">
@@ -930,80 +1004,96 @@
         <v>2</v>
       </c>
       <c r="L22" s="3">
-        <f>(F22-$D$19)/G22</f>
+        <f>(F22-$C$19)/H22</f>
         <v>4.4075983260119913E-4</v>
       </c>
       <c r="M22" s="3">
-        <f>SQRT(((1/(F4^2*G22))*G4)^2+((1/($D$8^2*G22))*$E$8)^2)</f>
+        <f>SQRT(((1/(F4^2*H22))*G4)^2+((1/($D$8^2*H22))*$E$8)^2)</f>
         <v>3.5746379753312753E-10</v>
       </c>
       <c r="N22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D23">
+      <c r="C23" s="4">
         <f>1/D5</f>
         <v>2.3187437973603421E-3</v>
       </c>
-      <c r="E23">
+      <c r="D23" s="4">
+        <f t="shared" si="2"/>
+        <v>1.5624320550398255E-9</v>
+      </c>
+      <c r="E23" s="4">
         <f>K5</f>
         <v>4</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="5">
         <f>1/F5</f>
         <v>2.9254307696808357E-3</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="5">
+        <f t="shared" si="3"/>
+        <v>1.0509402291103959E-9</v>
+      </c>
+      <c r="H23" s="5">
         <v>4</v>
       </c>
       <c r="I23" s="2">
-        <f>(D23-$D$19)/E23</f>
+        <f>(C23-$C$19)/E23</f>
         <v>4.660216862937014E-4</v>
       </c>
       <c r="J23" s="2">
-        <f t="shared" si="2"/>
+        <f>SQRT(((1/(D5^2*E23))*E5)^2+((1/($D$8^2*E23))*$E$8)^2)</f>
         <v>4.2076714849916516E-10</v>
       </c>
       <c r="K23">
         <v>4</v>
       </c>
       <c r="L23" s="3">
-        <f>(F23-$D$19)/G23</f>
+        <f>(F23-$C$19)/H23</f>
         <v>6.1769342937382479E-4</v>
       </c>
       <c r="M23" s="3">
-        <f>SQRT(((1/(F5^2*G23))*G5)^2+((1/($D$8^2*G23))*$E$8)^2)</f>
+        <f>SQRT(((1/(F5^2*H23))*G5)^2+((1/($D$8^2*H23))*$E$8)^2)</f>
         <v>3.0577783301816275E-10</v>
       </c>
       <c r="N23">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B24" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D24">
+      <c r="C24" s="4">
         <f>1/D12</f>
         <v>8.4869470753980375E-4</v>
       </c>
-      <c r="E24">
+      <c r="D24" s="4">
+        <f>(1/D12^2)*E12</f>
+        <v>7.0594908074461223E-10</v>
+      </c>
+      <c r="E24" s="4">
         <f>K6</f>
         <v>0.05</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="5">
         <f>1/F12</f>
         <v>1.823696011759192E-3</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="5">
+        <f>(1/F12^2)*G12</f>
+        <v>4.1839408662794293E-10</v>
+      </c>
+      <c r="H24" s="5">
         <v>0.05</v>
       </c>
       <c r="I24" s="2">
-        <f>(D24-$D$19)/E24</f>
+        <f>(C24-$C$19)/E24</f>
         <v>7.8807531070853448E-3</v>
       </c>
       <c r="J24" s="2">
@@ -1014,80 +1104,96 @@
         <v>0.05</v>
       </c>
       <c r="L24" s="3">
-        <f>(F24-$D$19)/G24</f>
+        <f>(F24-$C$19)/H24</f>
         <v>2.7380779191473109E-2</v>
       </c>
       <c r="M24" s="3">
-        <f>SQRT(((1/(F12^2*G24))*G12)^2+((1/($D$8^2*G24))*$E$8)^2)</f>
+        <f>SQRT(((1/(F12^2*H24))*G12)^2+((1/($D$8^2*H24))*$E$8)^2)</f>
         <v>1.5054296093901615E-8</v>
       </c>
       <c r="N24">
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B25" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D25">
+      <c r="C25" s="4">
         <f>1/D13</f>
         <v>1.3776818298921138E-3</v>
       </c>
-      <c r="E25">
+      <c r="D25" s="4">
+        <f t="shared" ref="D25:D27" si="4">(1/D13^2)*E13</f>
+        <v>1.1439289541548499E-9</v>
+      </c>
+      <c r="E25" s="4">
         <f>K7</f>
         <v>0.1</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="5">
         <f>1/F13</f>
         <v>3.5732407149340023E-3</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="5">
+        <f t="shared" ref="G25:G27" si="5">(1/F13^2)*G13</f>
+        <v>1.044298744629248E-9</v>
+      </c>
+      <c r="H25" s="5">
         <v>0.1</v>
       </c>
       <c r="I25" s="2">
-        <f>(D25-$D$19)/E25</f>
+        <f>(C25-$C$19)/E25</f>
         <v>9.2302477770657716E-3</v>
       </c>
       <c r="J25" s="2">
-        <f t="shared" ref="J25:J27" si="3">SQRT(((1/(D13^2*E25))*E13)^2+((1/($D$8^2*E25))*$E$8)^2)</f>
+        <f>SQRT(((1/(D13^2*E25))*E13)^2+((1/($D$8^2*E25))*$E$8)^2)</f>
         <v>1.3038786054060905E-8</v>
       </c>
       <c r="K25">
         <v>0.1</v>
       </c>
       <c r="L25" s="3">
-        <f>(F25-$D$19)/G25</f>
+        <f>(F25-$C$19)/H25</f>
         <v>3.1185836627484656E-2</v>
       </c>
       <c r="M25" s="3">
-        <f>SQRT(((1/(F13^2*G25))*G13)^2+((1/($D$8^2*G25))*$E$8)^2)</f>
+        <f>SQRT(((1/(F13^2*H25))*G13)^2+((1/($D$8^2*H25))*$E$8)^2)</f>
         <v>1.2174094765181295E-8</v>
       </c>
       <c r="N25">
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B26" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D26">
+      <c r="C26" s="4">
         <f>1/D14</f>
         <v>3.1637059651675975E-3</v>
       </c>
-      <c r="E26">
+      <c r="D26" s="4">
+        <f t="shared" si="4"/>
+        <v>3.081782010140005E-9</v>
+      </c>
+      <c r="E26" s="4">
         <f>K8</f>
         <v>0.2</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="5">
         <f>1/F14</f>
         <v>5.8480900138014923E-3</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="5">
+        <f t="shared" si="5"/>
+        <v>4.0424585348858233E-9</v>
+      </c>
+      <c r="H26" s="5">
         <v>0.2</v>
       </c>
       <c r="I26" s="2">
-        <f>(D26-$D$19)/E26</f>
+        <f>(C26-$C$19)/E26</f>
         <v>1.3545244564910304E-2</v>
       </c>
       <c r="J26" s="2">
@@ -1098,53 +1204,61 @@
         <v>0.2</v>
       </c>
       <c r="L26" s="3">
-        <f>(F26-$D$19)/G26</f>
+        <f>(F26-$C$19)/H26</f>
         <v>2.6967164808079779E-2</v>
       </c>
       <c r="M26" s="3">
-        <f>SQRT(((1/(F14^2*G26))*G14)^2+((1/($D$8^2*G26))*$E$8)^2)</f>
+        <f>SQRT(((1/(F14^2*H26))*G14)^2+((1/($D$8^2*H26))*$E$8)^2)</f>
         <v>2.0452993039988772E-8</v>
       </c>
       <c r="N26">
         <v>0.2</v>
       </c>
     </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B27" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D27">
+      <c r="C27" s="4">
         <f>1/D15</f>
         <v>5.5480348860433631E-3</v>
       </c>
-      <c r="E27">
+      <c r="D27" s="4">
+        <f t="shared" si="4"/>
+        <v>3.9214600457264849E-9</v>
+      </c>
+      <c r="E27" s="4">
         <f>K9</f>
         <v>0.4</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="5">
         <f>1/F15</f>
         <v>1.446106502851722E-2</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="5">
+        <f t="shared" si="5"/>
+        <v>1.1438995376217504E-8</v>
+      </c>
+      <c r="H27" s="5">
         <v>0.4</v>
       </c>
       <c r="I27" s="2">
-        <f>(D27-$D$19)/E27</f>
+        <f>(C27-$C$19)/E27</f>
         <v>1.2733444584644567E-2</v>
       </c>
       <c r="J27" s="2">
-        <f t="shared" si="3"/>
+        <f>SQRT(((1/(D15^2*E27))*E15)^2+((1/($D$8^2*E27))*$E$8)^2)</f>
         <v>9.9276680468372986E-9</v>
       </c>
       <c r="K27">
         <v>0.4</v>
       </c>
       <c r="L27" s="3">
-        <f>(F27-$D$19)/G27</f>
+        <f>(F27-$C$19)/H27</f>
         <v>3.5016019940829209E-2</v>
       </c>
       <c r="M27" s="3">
-        <f>SQRT(((1/(F15^2*G27))*G15)^2+((1/($D$8^2*G27))*$E$8)^2)</f>
+        <f>SQRT(((1/(F15^2*H27))*G15)^2+((1/($D$8^2*H27))*$E$8)^2)</f>
         <v>2.8640240613362452E-8</v>
       </c>
       <c r="N27">

</xml_diff>

<commit_message>
fehler in meiner auswertung
</commit_message>
<xml_diff>
--- a/Auswertung-MR/Excel/T1T2-Zeiten.xlsx
+++ b/Auswertung-MR/Excel/T1T2-Zeiten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Dokumente\Studium\Konstanz\7. Semester\FP\EFNMR-Remote\Auswertung-MR\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF87E255-EC0F-4F8B-AEBE-AEABC4320503}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E649B6E5-85C2-4213-A701-EFBC3E9F0ED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2232" yWindow="1560" windowWidth="12084" windowHeight="7920" xr2:uid="{A3CF1ACE-D739-42DC-9CD4-6918666B986E}"/>
+    <workbookView xWindow="1740" yWindow="1080" windowWidth="12084" windowHeight="7920" xr2:uid="{A3CF1ACE-D739-42DC-9CD4-6918666B986E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
   <si>
     <t>Relaxationszeiten</t>
   </si>
@@ -541,15 +541,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317E1452-D344-4788-8BB8-D10CA50AF815}">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="F26" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
@@ -587,16 +587,17 @@
         <v>3</v>
       </c>
       <c r="D2">
-        <v>1394.84</v>
+        <v>1.3948400000000001</v>
       </c>
       <c r="E2">
-        <v>1.0549999999999999E-3</v>
+        <f>0.001055/1000</f>
+        <v>1.0549999999999999E-6</v>
       </c>
       <c r="F2">
-        <v>1215.51</v>
+        <v>1.2155100000000001</v>
       </c>
       <c r="G2">
-        <v>2.5290000000000002E-4</v>
+        <v>2.5289999999999999E-7</v>
       </c>
       <c r="I2" t="s">
         <v>25</v>
@@ -618,16 +619,17 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>1003.4</v>
+        <v>1.0034000000000001</v>
       </c>
       <c r="E3">
-        <v>4.8509999999999997E-4</v>
+        <f>0.0004851/1000</f>
+        <v>4.8510000000000002E-7</v>
       </c>
       <c r="F3">
-        <v>1066.44</v>
+        <v>1.0664400000000001</v>
       </c>
       <c r="G3">
-        <v>2.6209999999999997E-4</v>
+        <v>2.621E-7</v>
       </c>
       <c r="J3">
         <f>500*10^(-6)</f>
@@ -643,16 +645,17 @@
         <v>5</v>
       </c>
       <c r="D4">
-        <v>646.84900000000005</v>
+        <v>0.64684900000000001</v>
       </c>
       <c r="E4">
-        <v>71.540000000000006</v>
+        <f>71.54/1000</f>
+        <v>7.1540000000000006E-2</v>
       </c>
       <c r="F4">
-        <v>748.404</v>
+        <v>0.74840399999999996</v>
       </c>
       <c r="G4">
-        <v>1.9369999999999999E-4</v>
+        <v>1.9369999999999999E-7</v>
       </c>
       <c r="J4">
         <f>1000*10^(-6)</f>
@@ -668,16 +671,17 @@
         <v>13</v>
       </c>
       <c r="D5">
-        <v>431.26799999999997</v>
+        <v>0.43126799999999998</v>
       </c>
       <c r="E5">
-        <v>2.9060000000000002E-4</v>
+        <f>0.0002906/1000</f>
+        <v>2.9060000000000002E-7</v>
       </c>
       <c r="F5">
-        <v>341.83</v>
+        <v>0.34183000000000002</v>
       </c>
       <c r="G5">
-        <v>1.228E-4</v>
+        <v>1.2279999999999999E-7</v>
       </c>
       <c r="J5">
         <f>2000*10^(-6)</f>
@@ -728,16 +732,16 @@
         <v>8</v>
       </c>
       <c r="D8">
-        <v>2199.46</v>
+        <v>2.1994600000000002</v>
       </c>
       <c r="E8">
-        <v>3.0270000000000002E-3</v>
+        <v>3.027E-6</v>
       </c>
       <c r="F8">
-        <v>1901.06</v>
+        <v>1.90106</v>
       </c>
       <c r="G8">
-        <v>89.83</v>
+        <v>8.9829999999999993E-2</v>
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
@@ -777,16 +781,16 @@
         <v>9</v>
       </c>
       <c r="D12">
-        <v>1178.28</v>
+        <v>1.17828</v>
       </c>
       <c r="E12">
-        <v>9.8010000000000002E-4</v>
+        <v>9.8009999999999994E-7</v>
       </c>
       <c r="F12">
-        <v>548.33699999999999</v>
+        <v>0.54833699999999996</v>
       </c>
       <c r="G12">
-        <v>1.2579999999999999E-4</v>
+        <v>1.258E-7</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -794,17 +798,17 @@
         <v>10</v>
       </c>
       <c r="D13">
-        <v>725.85699999999997</v>
+        <v>0.72585699999999997</v>
       </c>
       <c r="E13">
-        <v>6.0269999999999996E-4</v>
+        <v>6.0269999999999996E-7</v>
       </c>
       <c r="F13">
-        <v>279.858</v>
+        <v>0.279858</v>
       </c>
       <c r="G13">
-        <f>8.179*10^(-5)</f>
-        <v>8.1790000000000015E-5</v>
+        <f>8.179*10^(-8)</f>
+        <v>8.1790000000000006E-8</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -812,16 +816,16 @@
         <v>11</v>
       </c>
       <c r="D14">
-        <v>316.08499999999998</v>
+        <v>0.316085</v>
       </c>
       <c r="E14">
-        <v>3.079E-4</v>
+        <v>3.079E-7</v>
       </c>
       <c r="F14">
-        <v>170.99600000000001</v>
+        <v>0.17099600000000001</v>
       </c>
       <c r="G14">
-        <v>1.182E-4</v>
+        <v>1.182E-7</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -829,17 +833,17 @@
         <v>12</v>
       </c>
       <c r="D15">
-        <v>180.244</v>
+        <v>0.18024399999999999</v>
       </c>
       <c r="E15">
-        <v>1.2740000000000001E-4</v>
+        <v>1.2739999999999999E-7</v>
       </c>
       <c r="F15">
-        <v>69.151200000000003</v>
+        <v>6.9151199999999996E-2</v>
       </c>
       <c r="G15">
-        <f>5.47*10^(-5)</f>
-        <v>5.4700000000000001E-5</v>
+        <f>5.47*10^(-8)</f>
+        <v>5.47E-8</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -887,20 +891,20 @@
       </c>
       <c r="C19" s="4">
         <f>1/D8</f>
-        <v>4.5465705218553646E-4</v>
+        <v>0.45465705218553643</v>
       </c>
       <c r="D19" s="4">
         <f>(1/D8^2)*E8</f>
-        <v>6.2572035725388004E-10</v>
+        <v>6.2572035725387985E-7</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="5">
         <f>1/F8</f>
-        <v>5.2602232438744704E-4</v>
+        <v>0.526022324387447</v>
       </c>
       <c r="G19" s="5">
         <f>(1/F8^2)*G8</f>
-        <v>2.4855914805279351E-5</v>
+        <v>2.485591480527935E-2</v>
       </c>
       <c r="H19" s="5"/>
     </row>
@@ -910,11 +914,11 @@
       </c>
       <c r="C20" s="4">
         <f>1/D2</f>
-        <v>7.1692810644948533E-4</v>
+        <v>0.71692810644948524</v>
       </c>
       <c r="D20" s="4">
         <f>(1/D2^2)*E2</f>
-        <v>5.4225513485719294E-10</v>
+        <v>5.4225513485719275E-7</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" ref="E20:E27" si="2">K2</f>
@@ -922,33 +926,33 @@
       </c>
       <c r="F20" s="5">
         <f>1/F2</f>
-        <v>8.2269993665210492E-4</v>
+        <v>0.82269993665210484</v>
       </c>
       <c r="G20" s="5">
         <f>(1/F2^2)*G2</f>
-        <v>1.7117161848056976E-10</v>
+        <v>1.7117161848056968E-7</v>
       </c>
       <c r="H20" s="5">
         <v>0.5</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" ref="I20:I27" si="3">(C20-$C$19)/E20</f>
-        <v>5.2454210852789774E-4</v>
+        <v>0.52454210852789762</v>
       </c>
       <c r="J20" s="2">
         <f>SQRT(((1/(D2^2*E20))*E2)^2+((1/($D$8^2*E20))*$E$8)^2)</f>
-        <v>1.6559789814619215E-9</v>
+        <v>1.6559789814619209E-6</v>
       </c>
       <c r="K20">
         <v>0.5</v>
       </c>
       <c r="L20" s="3">
         <f t="shared" ref="L20:L27" si="4">(F20-$C$19)/H20</f>
-        <v>7.3608576893313693E-4</v>
+        <v>0.73608576893313682</v>
       </c>
       <c r="M20" s="3">
         <f>SQRT(((1/(F2^2*H20))*G2)^2+((1/($D$8^2*H20))*$E$8)^2)</f>
-        <v>1.2974215790639232E-9</v>
+        <v>1.2974215790639227E-6</v>
       </c>
       <c r="N20">
         <v>0.5</v>
@@ -960,11 +964,11 @@
       </c>
       <c r="C21" s="4">
         <f>1/D3</f>
-        <v>9.9661152082918089E-4</v>
+        <v>0.9966115208291807</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" ref="D21:D23" si="5">(1/D3^2)*E3</f>
-        <v>4.8181806732532946E-10</v>
+        <v>4.8181806732532946E-7</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="2"/>
@@ -972,33 +976,33 @@
       </c>
       <c r="F21" s="5">
         <f>1/F3</f>
-        <v>9.3769926109298226E-4</v>
+        <v>0.93769926109298218</v>
       </c>
       <c r="G21" s="5">
         <f t="shared" ref="G21:G23" si="6">(1/F3^2)*G3</f>
-        <v>2.304592629050585E-10</v>
+        <v>2.3045926290505855E-7</v>
       </c>
       <c r="H21" s="5">
         <v>1</v>
       </c>
       <c r="I21" s="2">
         <f t="shared" si="3"/>
-        <v>5.4195446864364438E-4</v>
+        <v>0.54195446864364427</v>
       </c>
       <c r="J21" s="2">
         <f>SQRT(((1/(D3^2*E21))*E3)^2+((1/($D$8^2*E21))*$E$8)^2)</f>
-        <v>7.8973072340072915E-10</v>
+        <v>7.8973072340072906E-7</v>
       </c>
       <c r="K21">
         <v>1</v>
       </c>
       <c r="L21" s="3">
         <f t="shared" si="4"/>
-        <v>4.830422089074458E-4</v>
+        <v>0.48304220890744576</v>
       </c>
       <c r="M21" s="3">
         <f>SQRT(((1/(F3^2*H21))*G3)^2+((1/($D$8^2*H21))*$E$8)^2)</f>
-        <v>6.6681139562897853E-10</v>
+        <v>6.6681139562897835E-7</v>
       </c>
       <c r="N21">
         <v>1</v>
@@ -1010,11 +1014,11 @@
       </c>
       <c r="C22" s="4">
         <f>1/D4</f>
-        <v>1.5459558567764654E-3</v>
+        <v>1.5459558567764655</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="5"/>
-        <v>1.7097913422419814E-4</v>
+        <v>0.17097913422419816</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="2"/>
@@ -1022,33 +1026,33 @@
       </c>
       <c r="F22" s="5">
         <f>1/F4</f>
-        <v>1.3361767173879348E-3</v>
+        <v>1.3361767173879349</v>
       </c>
       <c r="G22" s="5">
         <f t="shared" si="6"/>
-        <v>3.4582582423135492E-10</v>
+        <v>3.4582582423135504E-7</v>
       </c>
       <c r="H22" s="5">
         <v>2</v>
       </c>
       <c r="I22" s="2">
         <f t="shared" si="3"/>
-        <v>5.4564940229546446E-4</v>
+        <v>0.54564940229546455</v>
       </c>
       <c r="J22" s="2">
         <f>SQRT(((1/(D4^2*E22))*E4)^2+((1/($D$8^2*E22))*$E$8)^2)</f>
-        <v>8.5489567112671542E-5</v>
+        <v>8.5489567112671569E-2</v>
       </c>
       <c r="K22">
         <v>2</v>
       </c>
       <c r="L22" s="3">
         <f t="shared" si="4"/>
-        <v>4.4075983260119913E-4</v>
+        <v>0.44075983260119922</v>
       </c>
       <c r="M22" s="3">
         <f>SQRT(((1/(F4^2*H22))*G4)^2+((1/($D$8^2*H22))*$E$8)^2)</f>
-        <v>3.5746379753312753E-10</v>
+        <v>3.5746379753312755E-7</v>
       </c>
       <c r="N22">
         <v>2</v>
@@ -1060,11 +1064,11 @@
       </c>
       <c r="C23" s="4">
         <f>1/D5</f>
-        <v>2.3187437973603421E-3</v>
+        <v>2.3187437973603422</v>
       </c>
       <c r="D23" s="4">
         <f t="shared" si="5"/>
-        <v>1.5624320550398255E-9</v>
+        <v>1.5624320550398258E-6</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="2"/>
@@ -1072,33 +1076,33 @@
       </c>
       <c r="F23" s="5">
         <f>1/F5</f>
-        <v>2.9254307696808357E-3</v>
+        <v>2.9254307696808355</v>
       </c>
       <c r="G23" s="5">
         <f t="shared" si="6"/>
-        <v>1.0509402291103959E-9</v>
+        <v>1.0509402291103954E-6</v>
       </c>
       <c r="H23" s="5">
         <v>4</v>
       </c>
       <c r="I23" s="2">
         <f t="shared" si="3"/>
-        <v>4.660216862937014E-4</v>
+        <v>0.46602168629370144</v>
       </c>
       <c r="J23" s="2">
         <f>SQRT(((1/(D5^2*E23))*E5)^2+((1/($D$8^2*E23))*$E$8)^2)</f>
-        <v>4.2076714849916516E-10</v>
+        <v>4.207671484991652E-7</v>
       </c>
       <c r="K23">
         <v>4</v>
       </c>
       <c r="L23" s="3">
         <f t="shared" si="4"/>
-        <v>6.1769342937382479E-4</v>
+        <v>0.61769342937382476</v>
       </c>
       <c r="M23" s="3">
         <f>SQRT(((1/(F5^2*H23))*G5)^2+((1/($D$8^2*H23))*$E$8)^2)</f>
-        <v>3.0577783301816275E-10</v>
+        <v>3.0577783301816261E-7</v>
       </c>
       <c r="N23">
         <v>4</v>
@@ -1110,11 +1114,11 @@
       </c>
       <c r="C24" s="4">
         <f>1/D12</f>
-        <v>8.4869470753980375E-4</v>
+        <v>0.84869470753980381</v>
       </c>
       <c r="D24" s="4">
         <f>(1/D12^2)*E12</f>
-        <v>7.0594908074461223E-10</v>
+        <v>7.059490807446122E-7</v>
       </c>
       <c r="E24" s="4">
         <f t="shared" si="2"/>
@@ -1122,33 +1126,33 @@
       </c>
       <c r="F24" s="5">
         <f>1/F12</f>
-        <v>1.823696011759192E-3</v>
+        <v>1.823696011759192</v>
       </c>
       <c r="G24" s="5">
         <f>(1/F12^2)*G12</f>
-        <v>4.1839408662794293E-10</v>
+        <v>4.1839408662794298E-7</v>
       </c>
       <c r="H24" s="5">
         <v>0.05</v>
       </c>
       <c r="I24" s="2">
         <f t="shared" si="3"/>
-        <v>7.8807531070853448E-3</v>
+        <v>7.8807531070853472</v>
       </c>
       <c r="J24" s="2">
         <f>SQRT(((1/(D12^2*E24))*E12)^2+((1/($D$8^2*E24))*$E$8)^2)</f>
-        <v>1.8866796973371882E-8</v>
+        <v>1.8866796973371882E-5</v>
       </c>
       <c r="K24">
         <v>0.05</v>
       </c>
       <c r="L24" s="3">
         <f t="shared" si="4"/>
-        <v>2.7380779191473109E-2</v>
+        <v>27.38077919147311</v>
       </c>
       <c r="M24" s="3">
         <f>SQRT(((1/(F12^2*H24))*G12)^2+((1/($D$8^2*H24))*$E$8)^2)</f>
-        <v>1.5054296093901615E-8</v>
+        <v>1.5054296093901615E-5</v>
       </c>
       <c r="N24">
         <v>0.05</v>
@@ -1160,11 +1164,11 @@
       </c>
       <c r="C25" s="4">
         <f>1/D13</f>
-        <v>1.3776818298921138E-3</v>
+        <v>1.3776818298921139</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" ref="D25:D27" si="7">(1/D13^2)*E13</f>
-        <v>1.1439289541548499E-9</v>
+        <v>1.1439289541548501E-6</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="2"/>
@@ -1172,33 +1176,33 @@
       </c>
       <c r="F25" s="5">
         <f>1/F13</f>
-        <v>3.5732407149340023E-3</v>
+        <v>3.5732407149340024</v>
       </c>
       <c r="G25" s="5">
         <f t="shared" ref="G25:G27" si="8">(1/F13^2)*G13</f>
-        <v>1.044298744629248E-9</v>
+        <v>1.0442987446292479E-6</v>
       </c>
       <c r="H25" s="5">
         <v>0.1</v>
       </c>
       <c r="I25" s="2">
         <f t="shared" si="3"/>
-        <v>9.2302477770657716E-3</v>
+        <v>9.2302477770657738</v>
       </c>
       <c r="J25" s="2">
         <f>SQRT(((1/(D13^2*E25))*E13)^2+((1/($D$8^2*E25))*$E$8)^2)</f>
-        <v>1.3038786054060905E-8</v>
+        <v>1.3038786054060903E-5</v>
       </c>
       <c r="K25">
         <v>0.1</v>
       </c>
       <c r="L25" s="3">
         <f t="shared" si="4"/>
-        <v>3.1185836627484656E-2</v>
+        <v>31.185836627484658</v>
       </c>
       <c r="M25" s="3">
         <f>SQRT(((1/(F13^2*H25))*G13)^2+((1/($D$8^2*H25))*$E$8)^2)</f>
-        <v>1.2174094765181295E-8</v>
+        <v>1.2174094765181297E-5</v>
       </c>
       <c r="N25">
         <v>0.1</v>
@@ -1210,11 +1214,11 @@
       </c>
       <c r="C26" s="4">
         <f>1/D14</f>
-        <v>3.1637059651675975E-3</v>
+        <v>3.1637059651675972</v>
       </c>
       <c r="D26" s="4">
         <f t="shared" si="7"/>
-        <v>3.081782010140005E-9</v>
+        <v>3.081782010140004E-6</v>
       </c>
       <c r="E26" s="4">
         <f t="shared" si="2"/>
@@ -1222,33 +1226,33 @@
       </c>
       <c r="F26" s="5">
         <f>1/F14</f>
-        <v>5.8480900138014923E-3</v>
+        <v>5.8480900138014924</v>
       </c>
       <c r="G26" s="5">
         <f t="shared" si="8"/>
-        <v>4.0424585348858233E-9</v>
+        <v>4.0424585348858241E-6</v>
       </c>
       <c r="H26" s="5">
         <v>0.2</v>
       </c>
       <c r="I26" s="2">
         <f t="shared" si="3"/>
-        <v>1.3545244564910304E-2</v>
+        <v>13.545244564910304</v>
       </c>
       <c r="J26" s="2">
         <f>SQRT(((1/(D14^2*E26))*E14)^2+((1/($D$8^2*E26))*$E$8)^2)</f>
-        <v>1.5723315747246582E-8</v>
+        <v>1.5723315747246578E-5</v>
       </c>
       <c r="K26">
         <v>0.2</v>
       </c>
       <c r="L26" s="3">
         <f t="shared" si="4"/>
-        <v>2.6967164808079779E-2</v>
+        <v>26.967164808079776</v>
       </c>
       <c r="M26" s="3">
         <f>SQRT(((1/(F14^2*H26))*G14)^2+((1/($D$8^2*H26))*$E$8)^2)</f>
-        <v>2.0452993039988772E-8</v>
+        <v>2.0452993039988771E-5</v>
       </c>
       <c r="N26">
         <v>0.2</v>
@@ -1260,11 +1264,11 @@
       </c>
       <c r="C27" s="4">
         <f>1/D15</f>
-        <v>5.5480348860433631E-3</v>
+        <v>5.5480348860433635</v>
       </c>
       <c r="D27" s="4">
         <f t="shared" si="7"/>
-        <v>3.9214600457264849E-9</v>
+        <v>3.9214600457264852E-6</v>
       </c>
       <c r="E27" s="4">
         <f t="shared" si="2"/>
@@ -1272,33 +1276,33 @@
       </c>
       <c r="F27" s="5">
         <f>1/F15</f>
-        <v>1.446106502851722E-2</v>
+        <v>14.46106502851722</v>
       </c>
       <c r="G27" s="5">
         <f t="shared" si="8"/>
-        <v>1.1438995376217504E-8</v>
+        <v>1.1438995376217506E-5</v>
       </c>
       <c r="H27" s="5">
         <v>0.4</v>
       </c>
       <c r="I27" s="2">
         <f t="shared" si="3"/>
-        <v>1.2733444584644567E-2</v>
+        <v>12.733444584644568</v>
       </c>
       <c r="J27" s="2">
         <f>SQRT(((1/(D15^2*E27))*E15)^2+((1/($D$8^2*E27))*$E$8)^2)</f>
-        <v>9.9276680468372986E-9</v>
+        <v>9.927668046837299E-6</v>
       </c>
       <c r="K27">
         <v>0.4</v>
       </c>
       <c r="L27" s="3">
         <f t="shared" si="4"/>
-        <v>3.5016019940829209E-2</v>
+        <v>35.016019940829203</v>
       </c>
       <c r="M27" s="3">
         <f>SQRT(((1/(F15^2*H27))*G15)^2+((1/($D$8^2*H27))*$E$8)^2)</f>
-        <v>2.8640240613362452E-8</v>
+        <v>2.8640240613362459E-5</v>
       </c>
       <c r="N27">
         <v>0.4</v>
@@ -1431,6 +1435,135 @@
       <c r="M31" s="7">
         <f>(1/J31^2)*K31</f>
         <v>7480.1105736342706</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H33" t="s">
+        <v>31</v>
+      </c>
+      <c r="I33" t="s">
+        <v>36</v>
+      </c>
+      <c r="J33" t="s">
+        <v>40</v>
+      </c>
+      <c r="K33" t="s">
+        <v>41</v>
+      </c>
+      <c r="L33" t="s">
+        <v>33</v>
+      </c>
+      <c r="M33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="6">
+        <v>0.45395000000000002</v>
+      </c>
+      <c r="C34" s="6">
+        <v>3.0589999999999999E-2</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0.543404</v>
+      </c>
+      <c r="E34" s="6">
+        <v>7.0510000000000003E-2</v>
+      </c>
+      <c r="F34" s="7">
+        <f>1/D34</f>
+        <v>1.8402514519583957</v>
+      </c>
+      <c r="G34" s="7">
+        <f>(1/D34^2)*E34</f>
+        <v>0.23878390640773067</v>
+      </c>
+      <c r="H34" s="6">
+        <v>0.61660700000000002</v>
+      </c>
+      <c r="I34" s="7">
+        <v>8.3729999999999999E-2</v>
+      </c>
+      <c r="J34" s="6">
+        <v>0.34936299999999998</v>
+      </c>
+      <c r="K34" s="7">
+        <v>0.193</v>
+      </c>
+      <c r="L34" s="7">
+        <f>1/J34</f>
+        <v>2.8623523383987428</v>
+      </c>
+      <c r="M34" s="7">
+        <f>(1/J34^2)*K34</f>
+        <v>1.5812607554633933</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="6">
+        <v>13.6523</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0.83789999999999998</v>
+      </c>
+      <c r="D35" s="6">
+        <v>0.17471800000000001</v>
+      </c>
+      <c r="E35" s="6">
+        <v>0.19309999999999999</v>
+      </c>
+      <c r="F35" s="7">
+        <f>1/D35</f>
+        <v>5.723508739797845</v>
+      </c>
+      <c r="G35" s="7">
+        <f>(1/D35^2)*E35</f>
+        <v>6.3256764480761216</v>
+      </c>
+      <c r="H35" s="6">
+        <v>35.932699999999997</v>
+      </c>
+      <c r="I35" s="6">
+        <v>3.1360000000000001</v>
+      </c>
+      <c r="J35" s="6">
+        <v>-0.31085299999999999</v>
+      </c>
+      <c r="K35" s="6">
+        <v>0.7228</v>
+      </c>
+      <c r="L35" s="7">
+        <f>1/J35</f>
+        <v>-3.2169546377226537</v>
+      </c>
+      <c r="M35" s="7">
+        <f>(1/J35^2)*K35</f>
+        <v>7.4801105736342715</v>
       </c>
     </row>
   </sheetData>

</xml_diff>